<commit_message>
Capacidad del proyecto (Tiempos)
</commit_message>
<xml_diff>
--- a/Libro.xlsx
+++ b/Libro.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26930"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27002"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{92751763-BE84-4F35-A7A9-8766BFE7D49E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D9582E93-D00D-48AC-AA75-DE1A807880CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="110">
   <si>
     <t>Participante</t>
   </si>
@@ -139,7 +140,7 @@
     <t>Rest.</t>
   </si>
   <si>
-    <t>EP-01</t>
+    <t>EP-1</t>
   </si>
   <si>
     <t>Como usuario, se necesita añadir un producto con la finalidad de ponerlo en venta.</t>
@@ -154,7 +155,7 @@
     <t>Por iniciar</t>
   </si>
   <si>
-    <t>EP-02</t>
+    <t>EP-2</t>
   </si>
   <si>
     <t xml:space="preserve">Como usuario, se necesita marcar un artículo como favorito con la finalida de </t>
@@ -163,7 +164,7 @@
     <t>Añadir articulo a favoritos</t>
   </si>
   <si>
-    <t>EP-03</t>
+    <t>EP-3</t>
   </si>
   <si>
     <t>Como usuario, se necesita comentar un artículo con la finalidad de proporcionar una reseña del mismo</t>
@@ -172,7 +173,7 @@
     <t>Añadir comentario a un articulo</t>
   </si>
   <si>
-    <t>EP-04</t>
+    <t>EP-4</t>
   </si>
   <si>
     <t>Como usuario comprador, se necesita poder realizar una valoración del producto comprado con la finalidad de proporcionar feedback sobre el vendedor</t>
@@ -181,7 +182,7 @@
     <t>Valorar a un vendedor</t>
   </si>
   <si>
-    <t>EP-05</t>
+    <t>EP-5</t>
   </si>
   <si>
     <t>Como usuario, se necesita crear un perfil con la finalidad de identificarse con sus datos personales</t>
@@ -193,7 +194,7 @@
     <t>Por  iniciar</t>
   </si>
   <si>
-    <t>EP-06</t>
+    <t>EP-6</t>
   </si>
   <si>
     <t>Como usuario, necesito poder iniciar sesión para comprar y vender atículos</t>
@@ -202,7 +203,7 @@
     <t xml:space="preserve">Iniciar sesión </t>
   </si>
   <si>
-    <t>EP-07</t>
+    <t>EP-7</t>
   </si>
   <si>
     <t>Como usuario, se necesita cerrar una sesion iniciada con el fin de mantener la seguridad del perfil</t>
@@ -211,7 +212,7 @@
     <t>Cerrar sesion</t>
   </si>
   <si>
-    <t>EP-08</t>
+    <t>EP-8</t>
   </si>
   <si>
     <t>Como usuario, necesito consultar un artículo en concreto con la finalidad de visualizar toda la información acerca del producto.</t>
@@ -220,7 +221,7 @@
     <t>Consultar artículo</t>
   </si>
   <si>
-    <t>EP-09</t>
+    <t>EP-9</t>
   </si>
   <si>
     <t>Como vendedor, necesito modificar el artículo en venta con la finalidad de editar sus características</t>
@@ -293,13 +294,82 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Historia de usuario</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Tiempo disponible</t>
+  </si>
+  <si>
+    <t>40h50'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Tiempo utilizado por epico</t>
+  </si>
+  <si>
+    <t>26h</t>
+  </si>
+  <si>
+    <t>25h</t>
+  </si>
+  <si>
+    <t>22h</t>
+  </si>
+  <si>
+    <t>24h</t>
+  </si>
+  <si>
+    <t>Tiempo en reuniones</t>
+  </si>
+  <si>
+    <t>2h + 2h(Doc)</t>
+  </si>
+  <si>
+    <t>Tiempo productivo</t>
+  </si>
+  <si>
+    <t>32h36'</t>
+  </si>
+  <si>
+    <t>Tiempo final</t>
+  </si>
+  <si>
+    <t>30h</t>
+  </si>
+  <si>
+    <t>29h</t>
+  </si>
+  <si>
+    <t>28h</t>
+  </si>
+  <si>
+    <t>Tiempo sobrante</t>
+  </si>
+  <si>
+    <t>2h</t>
+  </si>
+  <si>
+    <t>3h</t>
+  </si>
+  <si>
+    <t>6h</t>
+  </si>
+  <si>
+    <t>4h</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -330,6 +400,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -351,7 +427,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -413,13 +489,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -434,12 +524,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -447,6 +531,22 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -763,8 +863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -857,7 +957,7 @@
       <c r="C4">
         <v>9</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4">
         <v>3</v>
       </c>
       <c r="E4">
@@ -902,8 +1002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EFCC409-402D-4C04-8FD5-6A2AF15AE81D}">
   <dimension ref="A1:V26"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -913,1065 +1013,1065 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="28.5">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
     </row>
     <row r="2" spans="1:22" ht="28.5">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
     </row>
     <row r="3" spans="1:22">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="8" t="s">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="9"/>
-      <c r="I3" s="8" t="s">
+      <c r="H3" s="11"/>
+      <c r="I3" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="9"/>
-      <c r="K3" s="8" t="s">
+      <c r="J3" s="11"/>
+      <c r="K3" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="9"/>
-      <c r="M3" s="8" t="s">
+      <c r="L3" s="11"/>
+      <c r="M3" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="9"/>
-      <c r="O3" s="8" t="s">
+      <c r="N3" s="11"/>
+      <c r="O3" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="8" t="s">
+      <c r="P3" s="11"/>
+      <c r="Q3" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="R3" s="9"/>
-      <c r="S3" s="8" t="s">
+      <c r="R3" s="11"/>
+      <c r="S3" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="T3" s="9"/>
-      <c r="U3" s="3"/>
-      <c r="V3" s="3"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
     </row>
     <row r="4" spans="1:22" ht="60.75">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="L4" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="M4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="N4" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="O4" s="5" t="s">
+      <c r="O4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="P4" s="5" t="s">
+      <c r="P4" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="Q4" s="5" t="s">
+      <c r="Q4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="R4" s="5" t="s">
+      <c r="R4" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="S4" s="5" t="s">
+      <c r="S4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="T4" s="5" t="s">
+      <c r="T4" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
     </row>
     <row r="5" spans="1:22" ht="45.75">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="12">
+        <v>15</v>
+      </c>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6">
+        <f>F5-G5</f>
+        <v>15</v>
+      </c>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6">
+        <f>H5-I5</f>
+        <v>15</v>
+      </c>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6">
+        <f>J5-K5</f>
+        <v>15</v>
+      </c>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6">
+        <f>L5-M5</f>
+        <v>15</v>
+      </c>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6">
+        <f>N5-O5</f>
+        <v>15</v>
+      </c>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6">
+        <f>P5-Q5</f>
+        <v>15</v>
+      </c>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6">
+        <f>R5-S5</f>
+        <v>15</v>
+      </c>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+    </row>
+    <row r="6" spans="1:22" ht="45.75">
+      <c r="A6" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="12">
+        <v>13</v>
+      </c>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6">
+        <f>F6-G6</f>
+        <v>13</v>
+      </c>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6">
+        <f>H6-I6</f>
+        <v>13</v>
+      </c>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6">
+        <f>J6-K6</f>
+        <v>13</v>
+      </c>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6">
+        <f>L6-M6</f>
+        <v>13</v>
+      </c>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6">
+        <f>N6-O6</f>
+        <v>13</v>
+      </c>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6">
+        <f>P6-Q6</f>
+        <v>13</v>
+      </c>
+      <c r="S6" s="6"/>
+      <c r="T6" s="6">
+        <f>R6-S6</f>
+        <v>13</v>
+      </c>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+    </row>
+    <row r="7" spans="1:22" ht="60.75">
+      <c r="A7" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="12">
         <v>9</v>
       </c>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7">
-        <f>F5-G5</f>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6">
+        <f>F7-G7</f>
         <v>9</v>
       </c>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7">
-        <f>H5-I5</f>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6">
+        <f>H7-I7</f>
         <v>9</v>
       </c>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7">
-        <f>J5-K5</f>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6">
+        <f>J7-K7</f>
         <v>9</v>
       </c>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7">
-        <f>L5-M5</f>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6">
+        <f>L7-M7</f>
         <v>9</v>
       </c>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7">
-        <f>N5-O5</f>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6">
+        <f>N7-O7</f>
         <v>9</v>
       </c>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7">
-        <f>P5-Q5</f>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6">
+        <f>P7-Q7</f>
         <v>9</v>
       </c>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7">
-        <f>R5-S5</f>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6">
+        <f>R7-S7</f>
         <v>9</v>
       </c>
-      <c r="U5" s="3"/>
-      <c r="V5" s="3"/>
-    </row>
-    <row r="6" spans="1:22" ht="45.75">
-      <c r="A6" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="6" t="s">
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+    </row>
+    <row r="8" spans="1:22" ht="91.5">
+      <c r="A8" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E8" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="6">
-        <v>7</v>
-      </c>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7">
-        <f>F6-G6</f>
-        <v>7</v>
-      </c>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7">
-        <f>H6-I6</f>
-        <v>7</v>
-      </c>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7">
-        <f>J6-K6</f>
-        <v>7</v>
-      </c>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7">
-        <f>L6-M6</f>
-        <v>7</v>
-      </c>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7">
-        <f>N6-O6</f>
-        <v>7</v>
-      </c>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7">
-        <f>P6-Q6</f>
-        <v>7</v>
-      </c>
-      <c r="S6" s="7"/>
-      <c r="T6" s="7">
-        <f>R6-S6</f>
-        <v>7</v>
-      </c>
-      <c r="U6" s="3"/>
-      <c r="V6" s="3"/>
-    </row>
-    <row r="7" spans="1:22" ht="60.75">
-      <c r="A7" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" s="6">
-        <v>6</v>
-      </c>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7">
-        <f>F7-G7</f>
-        <v>6</v>
-      </c>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7">
-        <f>H7-I7</f>
-        <v>6</v>
-      </c>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7">
-        <f>J7-K7</f>
-        <v>6</v>
-      </c>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7">
-        <f>L7-M7</f>
-        <v>6</v>
-      </c>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7">
-        <f>N7-O7</f>
-        <v>6</v>
-      </c>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7">
-        <f>P7-Q7</f>
-        <v>6</v>
-      </c>
-      <c r="S7" s="7"/>
-      <c r="T7" s="7">
-        <f>R7-S7</f>
-        <v>6</v>
-      </c>
-      <c r="U7" s="3"/>
-      <c r="V7" s="3"/>
-    </row>
-    <row r="8" spans="1:22" ht="91.5">
-      <c r="A8" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="6">
+      <c r="F8" s="12">
         <v>15</v>
       </c>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7">
+      <c r="G8" s="6"/>
+      <c r="H8" s="6">
         <f>F8-G8</f>
         <v>15</v>
       </c>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7">
+      <c r="I8" s="6"/>
+      <c r="J8" s="6">
         <f>H8-I8</f>
         <v>15</v>
       </c>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7">
+      <c r="K8" s="6"/>
+      <c r="L8" s="6">
         <f>J8-K8</f>
         <v>15</v>
       </c>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7">
+      <c r="M8" s="6"/>
+      <c r="N8" s="6">
         <f>L8-M8</f>
         <v>15</v>
       </c>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7">
+      <c r="O8" s="6"/>
+      <c r="P8" s="6">
         <f>N8-O8</f>
         <v>15</v>
       </c>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7">
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6">
         <f>P8-Q8</f>
         <v>15</v>
       </c>
-      <c r="S8" s="7"/>
-      <c r="T8" s="7">
+      <c r="S8" s="6"/>
+      <c r="T8" s="6">
         <f>R8-S8</f>
         <v>15</v>
       </c>
-      <c r="U8" s="3"/>
-      <c r="V8" s="3"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
     </row>
     <row r="9" spans="1:22" ht="60.75">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="F9" s="6">
-        <v>6</v>
-      </c>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7">
+      <c r="F9" s="12">
+        <v>11</v>
+      </c>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6">
         <f>F9-G9</f>
-        <v>6</v>
-      </c>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7">
+        <v>11</v>
+      </c>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6">
         <f>H9-I9</f>
-        <v>6</v>
-      </c>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7">
+        <v>11</v>
+      </c>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6">
         <f>J9-K9</f>
-        <v>6</v>
-      </c>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7">
+        <v>11</v>
+      </c>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6">
         <f>L9-M9</f>
-        <v>6</v>
-      </c>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7">
+        <v>11</v>
+      </c>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6">
         <f>N9-O9</f>
-        <v>6</v>
-      </c>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="7">
+        <v>11</v>
+      </c>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6">
         <f>P9-Q9</f>
-        <v>6</v>
-      </c>
-      <c r="S9" s="7"/>
-      <c r="T9" s="7">
+        <v>11</v>
+      </c>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6">
         <f>R9-S9</f>
-        <v>6</v>
-      </c>
-      <c r="U9" s="3"/>
-      <c r="V9" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
     </row>
     <row r="10" spans="1:22" ht="45.75">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F10" s="6">
-        <v>4</v>
-      </c>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7">
+      <c r="F10" s="12">
+        <v>8</v>
+      </c>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6">
         <f>F10-G10</f>
-        <v>4</v>
-      </c>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7">
+        <v>8</v>
+      </c>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6">
         <f>H10-I10</f>
-        <v>4</v>
-      </c>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7">
+        <v>8</v>
+      </c>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6">
         <f>J10-K10</f>
-        <v>4</v>
-      </c>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7">
+        <v>8</v>
+      </c>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6">
         <f>L10-M10</f>
-        <v>4</v>
-      </c>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7">
+        <v>8</v>
+      </c>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6">
         <f>N10-O10</f>
-        <v>4</v>
-      </c>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="7">
+        <v>8</v>
+      </c>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6">
         <f>P10-Q10</f>
-        <v>4</v>
-      </c>
-      <c r="S10" s="7"/>
-      <c r="T10" s="7">
+        <v>8</v>
+      </c>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6">
         <f>R10-S10</f>
-        <v>4</v>
-      </c>
-      <c r="U10" s="3"/>
-      <c r="V10" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
     </row>
     <row r="11" spans="1:22" ht="45.75">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="6">
-        <v>3</v>
-      </c>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7">
+      <c r="F11" s="12">
+        <v>8</v>
+      </c>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6">
         <f>F11-G11</f>
-        <v>3</v>
-      </c>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7">
+        <v>8</v>
+      </c>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6">
         <f>H11-I11</f>
-        <v>3</v>
-      </c>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7">
+        <v>8</v>
+      </c>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6">
         <f>J11-K11</f>
-        <v>3</v>
-      </c>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7">
+        <v>8</v>
+      </c>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6">
         <f>L11-M11</f>
-        <v>3</v>
-      </c>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7">
+        <v>8</v>
+      </c>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6">
         <f>N11-O11</f>
-        <v>3</v>
-      </c>
-      <c r="Q11" s="7"/>
-      <c r="R11" s="7">
+        <v>8</v>
+      </c>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6">
         <f>P11-Q11</f>
-        <v>3</v>
-      </c>
-      <c r="S11" s="7"/>
-      <c r="T11" s="7">
+        <v>8</v>
+      </c>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6">
         <f>R11-S11</f>
-        <v>3</v>
-      </c>
-      <c r="U11" s="3"/>
-      <c r="V11" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
     </row>
     <row r="12" spans="1:22" ht="60.75">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="6">
-        <v>6</v>
-      </c>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7">
+      <c r="F12" s="12">
+        <v>9</v>
+      </c>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6">
         <f>F12-G12</f>
-        <v>6</v>
-      </c>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7">
+        <v>9</v>
+      </c>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6">
         <f>H12-I12</f>
-        <v>6</v>
-      </c>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7">
+        <v>9</v>
+      </c>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6">
         <f>J12-K12</f>
-        <v>6</v>
-      </c>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7">
+        <v>9</v>
+      </c>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6">
         <f>L12-M12</f>
-        <v>6</v>
-      </c>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7">
+        <v>9</v>
+      </c>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6">
         <f>N12-O12</f>
-        <v>6</v>
-      </c>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="7">
+        <v>9</v>
+      </c>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6">
         <f>P12-Q12</f>
-        <v>6</v>
-      </c>
-      <c r="S12" s="7"/>
-      <c r="T12" s="7">
+        <v>9</v>
+      </c>
+      <c r="S12" s="6"/>
+      <c r="T12" s="6">
         <f>R12-S12</f>
-        <v>6</v>
-      </c>
-      <c r="U12" s="3"/>
-      <c r="V12" s="3"/>
+        <v>9</v>
+      </c>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
     </row>
     <row r="13" spans="1:22" ht="60.75">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="6">
-        <v>4</v>
-      </c>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7">
+      <c r="F13" s="12">
+        <v>8</v>
+      </c>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6">
         <f>F13-G13</f>
-        <v>4</v>
-      </c>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7">
+        <v>8</v>
+      </c>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6">
         <f>H13-I13</f>
-        <v>4</v>
-      </c>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7">
+        <v>8</v>
+      </c>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6">
         <f>J13-K13</f>
-        <v>4</v>
-      </c>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7">
+        <v>8</v>
+      </c>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6">
         <f>L13-M13</f>
-        <v>4</v>
-      </c>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7">
+        <v>8</v>
+      </c>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6">
         <f>N13-O13</f>
-        <v>4</v>
-      </c>
-      <c r="Q13" s="7"/>
-      <c r="R13" s="7">
+        <v>8</v>
+      </c>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6">
         <f>P13-Q13</f>
-        <v>4</v>
-      </c>
-      <c r="S13" s="7"/>
-      <c r="T13" s="7">
+        <v>8</v>
+      </c>
+      <c r="S13" s="6"/>
+      <c r="T13" s="6">
         <f>R13-S13</f>
-        <v>4</v>
-      </c>
-      <c r="U13" s="3"/>
-      <c r="V13" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
     </row>
     <row r="14" spans="1:22" ht="60.75">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F14" s="6">
-        <v>2</v>
-      </c>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7">
+      <c r="F14" s="12">
+        <v>8</v>
+      </c>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6">
         <f>F14-G14</f>
-        <v>2</v>
-      </c>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7">
+        <v>8</v>
+      </c>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6">
         <f>H14-I14</f>
-        <v>2</v>
-      </c>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7">
+        <v>8</v>
+      </c>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6">
         <f>J14-K14</f>
-        <v>2</v>
-      </c>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7">
+        <v>8</v>
+      </c>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6">
         <f>L14-M14</f>
-        <v>2</v>
-      </c>
-      <c r="O14" s="7"/>
-      <c r="P14" s="7">
+        <v>8</v>
+      </c>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6">
         <f>N14-O14</f>
-        <v>2</v>
-      </c>
-      <c r="Q14" s="7"/>
-      <c r="R14" s="7">
+        <v>8</v>
+      </c>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6">
         <f>P14-Q14</f>
-        <v>2</v>
-      </c>
-      <c r="S14" s="7"/>
-      <c r="T14" s="7">
+        <v>8</v>
+      </c>
+      <c r="S14" s="6"/>
+      <c r="T14" s="6">
         <f>R14-S14</f>
-        <v>2</v>
-      </c>
-      <c r="U14" s="3"/>
-      <c r="V14" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
     </row>
     <row r="15" spans="1:22" ht="76.5">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="6">
-        <v>2</v>
-      </c>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7">
+      <c r="F15" s="12">
+        <v>8</v>
+      </c>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6">
         <f>F15-G15</f>
-        <v>2</v>
-      </c>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7">
+        <v>8</v>
+      </c>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6">
         <f>H15-I15</f>
-        <v>2</v>
-      </c>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7">
+        <v>8</v>
+      </c>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6">
         <f>J15-K15</f>
-        <v>2</v>
-      </c>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7">
+        <v>8</v>
+      </c>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6">
         <f>L15-M15</f>
-        <v>2</v>
-      </c>
-      <c r="O15" s="7"/>
-      <c r="P15" s="7">
+        <v>8</v>
+      </c>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6">
         <f>N15-O15</f>
-        <v>2</v>
-      </c>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="7">
+        <v>8</v>
+      </c>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6">
         <f>P15-Q15</f>
-        <v>2</v>
-      </c>
-      <c r="S15" s="7"/>
-      <c r="T15" s="7">
+        <v>8</v>
+      </c>
+      <c r="S15" s="6"/>
+      <c r="T15" s="6">
         <f>R15-S15</f>
-        <v>2</v>
-      </c>
-      <c r="U15" s="3"/>
-      <c r="V15" s="3"/>
-    </row>
-    <row r="16" spans="1:22" s="11" customFormat="1" ht="57.75" customHeight="1">
-      <c r="A16" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="U15" s="2"/>
+      <c r="V15" s="2"/>
+    </row>
+    <row r="16" spans="1:22" s="8" customFormat="1" ht="57.75" customHeight="1">
+      <c r="A16" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="12">
         <v>24</v>
       </c>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7">
+      <c r="G16" s="6"/>
+      <c r="H16" s="6">
         <f>F16-G16</f>
         <v>24</v>
       </c>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7">
+      <c r="I16" s="6"/>
+      <c r="J16" s="6">
         <f>H16-I16</f>
         <v>24</v>
       </c>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7">
+      <c r="K16" s="6"/>
+      <c r="L16" s="6">
         <f>J16-K16</f>
         <v>24</v>
       </c>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7">
+      <c r="M16" s="6"/>
+      <c r="N16" s="6">
         <f>L16-M16</f>
         <v>24</v>
       </c>
-      <c r="O16" s="7"/>
-      <c r="P16" s="7">
+      <c r="O16" s="6"/>
+      <c r="P16" s="6">
         <f>N16-O16</f>
         <v>24</v>
       </c>
-      <c r="Q16" s="7"/>
-      <c r="R16" s="7">
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6">
         <f>P16-Q16</f>
         <v>24</v>
       </c>
-      <c r="S16" s="7"/>
-      <c r="T16" s="7">
+      <c r="S16" s="6"/>
+      <c r="T16" s="6">
         <f>R16-S16</f>
         <v>24</v>
       </c>
-      <c r="U16" s="10"/>
-      <c r="V16" s="10"/>
+      <c r="U16" s="7"/>
+      <c r="V16" s="7"/>
     </row>
     <row r="17" spans="1:22" ht="76.5">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="12">
         <v>9</v>
       </c>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7">
+      <c r="G17" s="6"/>
+      <c r="H17" s="6">
         <f>F17-G17</f>
         <v>9</v>
       </c>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7">
+      <c r="I17" s="6"/>
+      <c r="J17" s="6">
         <f>H17-I17</f>
         <v>9</v>
       </c>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7">
+      <c r="K17" s="6"/>
+      <c r="L17" s="6">
         <f>J17-K17</f>
         <v>9</v>
       </c>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7">
+      <c r="M17" s="6"/>
+      <c r="N17" s="6">
         <f>L17-M17</f>
         <v>9</v>
       </c>
-      <c r="O17" s="7"/>
-      <c r="P17" s="7">
+      <c r="O17" s="6"/>
+      <c r="P17" s="6">
         <f>N17-O17</f>
         <v>9</v>
       </c>
-      <c r="Q17" s="7"/>
-      <c r="R17" s="7">
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6">
         <f>P17-Q17</f>
         <v>9</v>
       </c>
-      <c r="S17" s="7"/>
-      <c r="T17" s="7">
+      <c r="S17" s="6"/>
+      <c r="T17" s="6">
         <f>R17-S17</f>
         <v>9</v>
       </c>
-      <c r="U17" s="3"/>
-      <c r="V17" s="3"/>
+      <c r="U17" s="2"/>
+      <c r="V17" s="2"/>
     </row>
     <row r="18" spans="1:22" ht="45.75">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="F18" s="6">
-        <v>4</v>
-      </c>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7">
+      <c r="F18" s="12">
+        <v>8</v>
+      </c>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6">
         <f>F18-G18</f>
-        <v>4</v>
-      </c>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7">
+        <v>8</v>
+      </c>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6">
         <f>H18-I18</f>
-        <v>4</v>
-      </c>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7">
+        <v>8</v>
+      </c>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6">
         <f>J18-K18</f>
-        <v>4</v>
-      </c>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7">
+        <v>8</v>
+      </c>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6">
         <f>L18-M18</f>
-        <v>4</v>
-      </c>
-      <c r="O18" s="7"/>
-      <c r="P18" s="7">
+        <v>8</v>
+      </c>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6">
         <f>N18-O18</f>
-        <v>4</v>
-      </c>
-      <c r="Q18" s="7"/>
-      <c r="R18" s="7">
+        <v>8</v>
+      </c>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6">
         <f>P18-Q18</f>
-        <v>4</v>
-      </c>
-      <c r="S18" s="7"/>
-      <c r="T18" s="7">
+        <v>8</v>
+      </c>
+      <c r="S18" s="6"/>
+      <c r="T18" s="6">
         <f>R18-S18</f>
-        <v>4</v>
-      </c>
-      <c r="U18" s="3"/>
-      <c r="V18" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
     </row>
     <row r="19" spans="1:22" ht="45.75">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="F19" s="6">
-        <v>3</v>
-      </c>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7">
+      <c r="F19" s="12">
+        <v>8</v>
+      </c>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6">
         <f>F19-G19</f>
-        <v>3</v>
-      </c>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7">
+        <v>8</v>
+      </c>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6">
         <f>H19-I19</f>
-        <v>3</v>
-      </c>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7">
+        <v>8</v>
+      </c>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6">
         <f>J19-K19</f>
-        <v>3</v>
-      </c>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7">
+        <v>8</v>
+      </c>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6">
         <f>L19-M19</f>
-        <v>3</v>
-      </c>
-      <c r="O19" s="7"/>
-      <c r="P19" s="7">
+        <v>8</v>
+      </c>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6">
         <f>N19-O19</f>
-        <v>3</v>
-      </c>
-      <c r="Q19" s="7"/>
-      <c r="R19" s="7">
+        <v>8</v>
+      </c>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6">
         <f>P19-Q19</f>
-        <v>3</v>
-      </c>
-      <c r="S19" s="7"/>
-      <c r="T19" s="7">
+        <v>8</v>
+      </c>
+      <c r="S19" s="6"/>
+      <c r="T19" s="6">
         <f>R19-S19</f>
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:22" ht="60.75">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E20" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="6">
-        <v>8</v>
-      </c>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7">
+      <c r="F20" s="12">
+        <v>11</v>
+      </c>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6">
         <f>F20-G20</f>
-        <v>8</v>
-      </c>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7">
+        <v>11</v>
+      </c>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6">
         <f>H20-I20</f>
-        <v>8</v>
-      </c>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7">
+        <v>11</v>
+      </c>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6">
         <f>J20-K20</f>
-        <v>8</v>
-      </c>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7">
+        <v>11</v>
+      </c>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6">
         <f>L20-M20</f>
-        <v>8</v>
-      </c>
-      <c r="O20" s="7"/>
-      <c r="P20" s="7">
+        <v>11</v>
+      </c>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6">
         <f>N20-O20</f>
-        <v>8</v>
-      </c>
-      <c r="Q20" s="7"/>
-      <c r="R20" s="7">
+        <v>11</v>
+      </c>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6">
         <f>P20-Q20</f>
-        <v>8</v>
-      </c>
-      <c r="S20" s="7"/>
-      <c r="T20" s="7">
+        <v>11</v>
+      </c>
+      <c r="S20" s="6"/>
+      <c r="T20" s="6">
         <f>R20-S20</f>
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:22">
@@ -1979,11 +2079,12 @@
         <v>86</v>
       </c>
       <c r="F21">
-        <v>112</v>
+        <f>SUM(F6:F20)</f>
+        <v>157</v>
       </c>
     </row>
     <row r="26" spans="1:22">
-      <c r="F26" s="12"/>
+      <c r="F26" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1997,4 +2098,438 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2A67B82-1C1F-433B-A4E4-B4AC96FCB4EE}">
+  <dimension ref="A2:I24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="26.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" ht="30" customHeight="1">
+      <c r="A2" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H8" s="14"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H9" s="14"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H13" s="14"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19" t="s">
+        <v>90</v>
+      </c>
+      <c r="C19" t="s">
+        <v>90</v>
+      </c>
+      <c r="D19" t="s">
+        <v>90</v>
+      </c>
+      <c r="E19" t="s">
+        <v>90</v>
+      </c>
+      <c r="F19" t="s">
+        <v>90</v>
+      </c>
+      <c r="G19" t="s">
+        <v>90</v>
+      </c>
+      <c r="H19" t="s">
+        <v>90</v>
+      </c>
+      <c r="I19" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" t="s">
+        <v>92</v>
+      </c>
+      <c r="B20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C20" t="s">
+        <v>94</v>
+      </c>
+      <c r="D20" t="s">
+        <v>94</v>
+      </c>
+      <c r="E20" t="s">
+        <v>93</v>
+      </c>
+      <c r="F20" t="s">
+        <v>95</v>
+      </c>
+      <c r="G20" t="s">
+        <v>96</v>
+      </c>
+      <c r="H20" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" t="s">
+        <v>97</v>
+      </c>
+      <c r="B21" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" t="s">
+        <v>98</v>
+      </c>
+      <c r="D21" t="s">
+        <v>98</v>
+      </c>
+      <c r="E21" t="s">
+        <v>98</v>
+      </c>
+      <c r="F21" t="s">
+        <v>98</v>
+      </c>
+      <c r="G21" t="s">
+        <v>98</v>
+      </c>
+      <c r="H21" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" t="s">
+        <v>99</v>
+      </c>
+      <c r="B22" t="s">
+        <v>100</v>
+      </c>
+      <c r="C22" t="s">
+        <v>100</v>
+      </c>
+      <c r="D22" t="s">
+        <v>100</v>
+      </c>
+      <c r="E22" t="s">
+        <v>100</v>
+      </c>
+      <c r="F22" t="s">
+        <v>100</v>
+      </c>
+      <c r="G22" t="s">
+        <v>100</v>
+      </c>
+      <c r="H22" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" t="s">
+        <v>101</v>
+      </c>
+      <c r="B23" t="s">
+        <v>102</v>
+      </c>
+      <c r="C23" t="s">
+        <v>103</v>
+      </c>
+      <c r="D23" t="s">
+        <v>103</v>
+      </c>
+      <c r="E23" t="s">
+        <v>102</v>
+      </c>
+      <c r="F23" t="s">
+        <v>93</v>
+      </c>
+      <c r="G23" t="s">
+        <v>104</v>
+      </c>
+      <c r="H23" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" t="s">
+        <v>105</v>
+      </c>
+      <c r="B24" t="s">
+        <v>106</v>
+      </c>
+      <c r="C24" t="s">
+        <v>107</v>
+      </c>
+      <c r="D24" t="s">
+        <v>107</v>
+      </c>
+      <c r="E24" t="s">
+        <v>106</v>
+      </c>
+      <c r="F24" t="s">
+        <v>108</v>
+      </c>
+      <c r="G24" t="s">
+        <v>109</v>
+      </c>
+      <c r="H24" t="s">
+        <v>109</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Cambio de RE a HU en ids
</commit_message>
<xml_diff>
--- a/Libro.xlsx
+++ b/Libro.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27002"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D9582E93-D00D-48AC-AA75-DE1A807880CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="521" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1DCE7A11-92FC-41D3-BE19-F769B0A5A510}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -140,7 +140,7 @@
     <t>Rest.</t>
   </si>
   <si>
-    <t>EP-1</t>
+    <t>HU-1</t>
   </si>
   <si>
     <t>Como usuario, se necesita añadir un producto con la finalidad de ponerlo en venta.</t>
@@ -155,7 +155,7 @@
     <t>Por iniciar</t>
   </si>
   <si>
-    <t>EP-2</t>
+    <t>HU-2</t>
   </si>
   <si>
     <t xml:space="preserve">Como usuario, se necesita marcar un artículo como favorito con la finalida de </t>
@@ -164,7 +164,7 @@
     <t>Añadir articulo a favoritos</t>
   </si>
   <si>
-    <t>EP-3</t>
+    <t>HU-3</t>
   </si>
   <si>
     <t>Como usuario, se necesita comentar un artículo con la finalidad de proporcionar una reseña del mismo</t>
@@ -173,7 +173,7 @@
     <t>Añadir comentario a un articulo</t>
   </si>
   <si>
-    <t>EP-4</t>
+    <t>HU-4</t>
   </si>
   <si>
     <t>Como usuario comprador, se necesita poder realizar una valoración del producto comprado con la finalidad de proporcionar feedback sobre el vendedor</t>
@@ -182,7 +182,7 @@
     <t>Valorar a un vendedor</t>
   </si>
   <si>
-    <t>EP-5</t>
+    <t>HU-5</t>
   </si>
   <si>
     <t>Como usuario, se necesita crear un perfil con la finalidad de identificarse con sus datos personales</t>
@@ -194,7 +194,7 @@
     <t>Por  iniciar</t>
   </si>
   <si>
-    <t>EP-6</t>
+    <t>HU-6</t>
   </si>
   <si>
     <t>Como usuario, necesito poder iniciar sesión para comprar y vender atículos</t>
@@ -203,7 +203,7 @@
     <t xml:space="preserve">Iniciar sesión </t>
   </si>
   <si>
-    <t>EP-7</t>
+    <t>HU-7</t>
   </si>
   <si>
     <t>Como usuario, se necesita cerrar una sesion iniciada con el fin de mantener la seguridad del perfil</t>
@@ -212,7 +212,7 @@
     <t>Cerrar sesion</t>
   </si>
   <si>
-    <t>EP-8</t>
+    <t>HU-8</t>
   </si>
   <si>
     <t>Como usuario, necesito consultar un artículo en concreto con la finalidad de visualizar toda la información acerca del producto.</t>
@@ -221,7 +221,7 @@
     <t>Consultar artículo</t>
   </si>
   <si>
-    <t>EP-9</t>
+    <t>HU-9</t>
   </si>
   <si>
     <t>Como vendedor, necesito modificar el artículo en venta con la finalidad de editar sus características</t>
@@ -230,7 +230,7 @@
     <t>Modificar articulo</t>
   </si>
   <si>
-    <t>EP-10</t>
+    <t>HU-10</t>
   </si>
   <si>
     <t>Como usuario vendedor, necesito poder eliminar el articulo en venta con el fin de quitarlo de la plataforma</t>
@@ -239,7 +239,7 @@
     <t>Borrar articulo</t>
   </si>
   <si>
-    <t>EP-11</t>
+    <t>HU-11</t>
   </si>
   <si>
     <t>Como usuario, necesito poder borrar un artículo seleccionado como favorito con la finalidad de no tenerlo en la sección de favoritos</t>
@@ -248,7 +248,7 @@
     <t>Borrar artículo de favoritos</t>
   </si>
   <si>
-    <t>EP-12</t>
+    <t>HU-12</t>
   </si>
   <si>
     <t>Como usuario, necesito realizar busquedas aplicando filtros para poder encontrar un artículo de forma rapida</t>
@@ -257,7 +257,7 @@
     <t>Busqueda avanzada con filtros</t>
   </si>
   <si>
-    <t>EP-13</t>
+    <t>HU-13</t>
   </si>
   <si>
     <t>Como usuario, necesito poder consultar el perfil de un vendedor con el fin de visualizar sus articulos en venta y su valoracion</t>
@@ -266,7 +266,7 @@
     <t>Consultar perfil con informacion</t>
   </si>
   <si>
-    <t>EP-14</t>
+    <t>HU-14</t>
   </si>
   <si>
     <t>Como usuario, necesito poder modificar mi perfil con el fin de editar mis datos</t>
@@ -275,7 +275,7 @@
     <t>Modificar perfil</t>
   </si>
   <si>
-    <t>EP-15</t>
+    <t>HU-15</t>
   </si>
   <si>
     <t>Como usuario, necesito poder borrar mi perfil con el fin de eliminarlo de la plataforma</t>
@@ -284,7 +284,7 @@
     <t>Borrar perfil</t>
   </si>
   <si>
-    <t>EP-16</t>
+    <t>HU-16</t>
   </si>
   <si>
     <t>Como usuario comprador, necesito comprar un artículo de segunda mano porque estoy interesado en obtenerlo</t>
@@ -407,7 +407,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -423,6 +423,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -508,7 +520,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -540,11 +552,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -864,7 +881,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1002,8 +1019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EFCC409-402D-4C04-8FD5-6A2AF15AE81D}">
   <dimension ref="A1:V26"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2102,10 +2119,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2A67B82-1C1F-433B-A4E4-B4AC96FCB4EE}">
-  <dimension ref="A2:I24"/>
+  <dimension ref="A2:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2121,411 +2138,421 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="30" customHeight="1">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="16" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14" t="s">
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14" t="s">
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14" t="s">
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14" t="s">
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="H8" s="14"/>
+      <c r="H8" s="13"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14" t="s">
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="H9" s="14"/>
+      <c r="H9" s="13"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14" t="s">
+      <c r="B11" s="13"/>
+      <c r="C11" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14" t="s">
+      <c r="B12" s="13"/>
+      <c r="C12" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14" t="s">
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="H13" s="14"/>
+      <c r="H13" s="13"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14" t="s">
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14" t="s">
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14" t="s">
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14" t="s">
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14" t="s">
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" t="s">
+      <c r="A19" s="14"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D20" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E20" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F20" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G20" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H20" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I20" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
-      <c r="A20" t="s">
+    <row r="21" spans="1:9">
+      <c r="A21" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D21" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E21" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F21" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G21" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H21" s="13" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
-      <c r="A21" t="s">
+    <row r="22" spans="1:9">
+      <c r="A22" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D22" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E22" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F22" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G22" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H22" s="13" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
-      <c r="A22" t="s">
+    <row r="23" spans="1:9">
+      <c r="A23" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D23" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E23" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F23" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G23" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H23" s="13" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
-      <c r="A23" t="s">
+    <row r="24" spans="1:9">
+      <c r="A24" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D24" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E24" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F24" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G24" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H24" s="13" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
-      <c r="A24" t="s">
+    <row r="25" spans="1:9">
+      <c r="A25" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D25" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E25" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F25" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G25" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H25" s="13" t="s">
         <v>109</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Planificación de excel terminada
</commit_message>
<xml_diff>
--- a/Libro.xlsx
+++ b/Libro.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27002"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="521" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1DCE7A11-92FC-41D3-BE19-F769B0A5A510}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{11EF8E83-F8B9-403B-B963-7FA9A05279CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="142">
   <si>
     <t>Participante</t>
   </si>
@@ -65,28 +65,37 @@
     <t>3h20'</t>
   </si>
   <si>
+    <t>16h40'</t>
+  </si>
+  <si>
     <t>Guillermo Dueñas Corraliza</t>
   </si>
   <si>
-    <t>SCRUM Master (50%): 90'</t>
+    <t>SCRUM Master (50%): 3h</t>
+  </si>
+  <si>
+    <t>15h</t>
+  </si>
+  <si>
+    <t>75h</t>
+  </si>
+  <si>
+    <t>Ismael Bocadulce Serrano</t>
+  </si>
+  <si>
+    <t>Desarrollador Senior (100%): 3h</t>
+  </si>
+  <si>
+    <t>Javier Rodriguez Mozo</t>
+  </si>
+  <si>
+    <t>Desarrollador Junior (100%): 90'</t>
   </si>
   <si>
     <t>7h30'</t>
   </si>
   <si>
-    <t>Ismael Bocadulce Serrano</t>
-  </si>
-  <si>
-    <t>Desarrollador Senior (100%): 3h</t>
-  </si>
-  <si>
-    <t>15h</t>
-  </si>
-  <si>
-    <t>Javier Rodriguez Mozo</t>
-  </si>
-  <si>
-    <t>Desarrollador Junior (100%): 3h</t>
+    <t>37h30'</t>
   </si>
   <si>
     <t>Metodologías ágiles - SCRUM: Lista de tareas de la iteración</t>
@@ -299,7 +308,94 @@
     <t>Historia de usuario</t>
   </si>
   <si>
-    <t>x</t>
+    <t>Leyenda:</t>
+  </si>
+  <si>
+    <t>PO:  3h</t>
+  </si>
+  <si>
+    <t>PO -&gt; Product Owner</t>
+  </si>
+  <si>
+    <t>DS: 12h</t>
+  </si>
+  <si>
+    <t>DS -&gt; Desarrollador Senior</t>
+  </si>
+  <si>
+    <t>PO: 2,6h</t>
+  </si>
+  <si>
+    <t>DJ -&gt; Desarrollador Junior</t>
+  </si>
+  <si>
+    <t>SM: 6,5h</t>
+  </si>
+  <si>
+    <t>SM -&gt; SCRUM Master</t>
+  </si>
+  <si>
+    <t>DS: 3,9h</t>
+  </si>
+  <si>
+    <t>DS: 6,3h</t>
+  </si>
+  <si>
+    <t>DJ: 2,7h</t>
+  </si>
+  <si>
+    <t>DJ: 7,5h</t>
+  </si>
+  <si>
+    <t>DS: 7,5h</t>
+  </si>
+  <si>
+    <t>DJ: 5,5h</t>
+  </si>
+  <si>
+    <t>SM: 5,5h</t>
+  </si>
+  <si>
+    <t>PO: 1,6h</t>
+  </si>
+  <si>
+    <t>SM: 4h</t>
+  </si>
+  <si>
+    <t>DS: 2,4h</t>
+  </si>
+  <si>
+    <t>DS: 8h</t>
+  </si>
+  <si>
+    <t>DS: 6,4h</t>
+  </si>
+  <si>
+    <t>DJ: 8h</t>
+  </si>
+  <si>
+    <t>SM: 4,5h</t>
+  </si>
+  <si>
+    <t>DS: 4,5h</t>
+  </si>
+  <si>
+    <t>DS: 9h</t>
+  </si>
+  <si>
+    <t>DJ: 15h</t>
+  </si>
+  <si>
+    <t>PO:1,8h</t>
+  </si>
+  <si>
+    <t>PO: 2,2h</t>
+  </si>
+  <si>
+    <t>SM: 4.4h</t>
+  </si>
+  <si>
+    <t>DS: 4,4h</t>
   </si>
   <si>
     <t>Tiempo disponible</t>
@@ -439,7 +535,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -516,11 +612,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -543,20 +676,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -564,6 +690,33 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -878,10 +1031,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -895,7 +1048,7 @@
     <col min="7" max="7" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -918,7 +1071,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -940,10 +1093,13 @@
       <c r="G2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -958,15 +1114,18 @@
         <v>6</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>5</v>
@@ -981,15 +1140,18 @@
         <v>6</v>
       </c>
       <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" t="s">
         <v>14</v>
       </c>
-      <c r="G4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5">
         <v>5</v>
@@ -1004,10 +1166,13 @@
         <v>7.5</v>
       </c>
       <c r="F5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G5" t="s">
-        <v>15</v>
+        <v>19</v>
+      </c>
+      <c r="H5" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1019,8 +1184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EFCC409-402D-4C04-8FD5-6A2AF15AE81D}">
   <dimension ref="A1:V26"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1031,7 +1196,7 @@
   <sheetData>
     <row r="1" spans="1:22" ht="28.5">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1057,7 +1222,7 @@
     </row>
     <row r="2" spans="1:22" ht="28.5">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1088,118 +1253,118 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="11"/>
-      <c r="I3" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="11"/>
-      <c r="K3" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" s="11"/>
-      <c r="M3" s="10" t="s">
+      <c r="G3" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="11"/>
-      <c r="O3" s="10" t="s">
+      <c r="H3" s="17"/>
+      <c r="I3" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="10" t="s">
+      <c r="J3" s="17"/>
+      <c r="K3" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="R3" s="11"/>
-      <c r="S3" s="10" t="s">
+      <c r="L3" s="17"/>
+      <c r="M3" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="T3" s="11"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="R3" s="17"/>
+      <c r="S3" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="T3" s="17"/>
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
     </row>
     <row r="4" spans="1:22" ht="60.75">
       <c r="A4" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="S4" s="4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="T4" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="U4" s="2"/>
       <c r="V4" s="2"/>
     </row>
     <row r="5" spans="1:22" ht="45.75">
       <c r="A5" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" s="12">
+        <v>42</v>
+      </c>
+      <c r="F5" s="10">
         <v>15</v>
       </c>
       <c r="G5" s="6"/>
@@ -1242,21 +1407,21 @@
     </row>
     <row r="6" spans="1:22" ht="45.75">
       <c r="A6" s="5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="E6" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" s="12">
+      <c r="F6" s="10">
         <v>13</v>
       </c>
       <c r="G6" s="6"/>
@@ -1299,21 +1464,21 @@
     </row>
     <row r="7" spans="1:22" ht="60.75">
       <c r="A7" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" s="12">
+        <v>42</v>
+      </c>
+      <c r="F7" s="10">
         <v>9</v>
       </c>
       <c r="G7" s="6"/>
@@ -1356,21 +1521,21 @@
     </row>
     <row r="8" spans="1:22" ht="91.5">
       <c r="A8" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="12">
+        <v>42</v>
+      </c>
+      <c r="F8" s="10">
         <v>15</v>
       </c>
       <c r="G8" s="6"/>
@@ -1413,21 +1578,21 @@
     </row>
     <row r="9" spans="1:22" ht="60.75">
       <c r="A9" s="5" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F9" s="12">
+        <v>55</v>
+      </c>
+      <c r="F9" s="10">
         <v>11</v>
       </c>
       <c r="G9" s="6"/>
@@ -1470,21 +1635,21 @@
     </row>
     <row r="10" spans="1:22" ht="45.75">
       <c r="A10" s="5" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F10" s="12">
+        <v>42</v>
+      </c>
+      <c r="F10" s="10">
         <v>8</v>
       </c>
       <c r="G10" s="6"/>
@@ -1527,21 +1692,21 @@
     </row>
     <row r="11" spans="1:22" ht="45.75">
       <c r="A11" s="5" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" s="12">
+        <v>42</v>
+      </c>
+      <c r="F11" s="10">
         <v>8</v>
       </c>
       <c r="G11" s="6"/>
@@ -1584,78 +1749,78 @@
     </row>
     <row r="12" spans="1:22" ht="60.75">
       <c r="A12" s="5" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F12" s="12">
-        <v>9</v>
+        <v>42</v>
+      </c>
+      <c r="F12" s="10">
+        <v>8</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="6">
         <f>F12-G12</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I12" s="6"/>
       <c r="J12" s="6">
         <f>H12-I12</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K12" s="6"/>
       <c r="L12" s="6">
         <f>J12-K12</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M12" s="6"/>
       <c r="N12" s="6">
         <f>L12-M12</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O12" s="6"/>
       <c r="P12" s="6">
         <f>N12-O12</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Q12" s="6"/>
       <c r="R12" s="6">
         <f>P12-Q12</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S12" s="6"/>
       <c r="T12" s="6">
         <f>R12-S12</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="U12" s="2"/>
       <c r="V12" s="2"/>
     </row>
     <row r="13" spans="1:22" ht="60.75">
       <c r="A13" s="5" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" s="12">
+        <v>42</v>
+      </c>
+      <c r="F13" s="10">
         <v>8</v>
       </c>
       <c r="G13" s="6"/>
@@ -1698,78 +1863,78 @@
     </row>
     <row r="14" spans="1:22" ht="60.75">
       <c r="A14" s="5" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F14" s="12">
-        <v>8</v>
+        <v>42</v>
+      </c>
+      <c r="F14" s="10">
+        <v>9</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="6">
         <f>F14-G14</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I14" s="6"/>
       <c r="J14" s="6">
         <f>H14-I14</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K14" s="6"/>
       <c r="L14" s="6">
         <f>J14-K14</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M14" s="6"/>
       <c r="N14" s="6">
         <f>L14-M14</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O14" s="6"/>
       <c r="P14" s="6">
         <f>N14-O14</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="Q14" s="6"/>
       <c r="R14" s="6">
         <f>P14-Q14</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S14" s="6"/>
       <c r="T14" s="6">
         <f>R14-S14</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
     </row>
     <row r="15" spans="1:22" ht="76.5">
       <c r="A15" s="5" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F15" s="12">
+        <v>42</v>
+      </c>
+      <c r="F15" s="10">
         <v>8</v>
       </c>
       <c r="G15" s="6"/>
@@ -1812,21 +1977,21 @@
     </row>
     <row r="16" spans="1:22" s="8" customFormat="1" ht="57.75" customHeight="1">
       <c r="A16" s="5" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F16" s="12">
+        <v>42</v>
+      </c>
+      <c r="F16" s="10">
         <v>24</v>
       </c>
       <c r="G16" s="6"/>
@@ -1869,21 +2034,21 @@
     </row>
     <row r="17" spans="1:22" ht="76.5">
       <c r="A17" s="5" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F17" s="12">
+        <v>55</v>
+      </c>
+      <c r="F17" s="10">
         <v>9</v>
       </c>
       <c r="G17" s="6"/>
@@ -1926,21 +2091,21 @@
     </row>
     <row r="18" spans="1:22" ht="45.75">
       <c r="A18" s="5" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F18" s="12">
+        <v>55</v>
+      </c>
+      <c r="F18" s="10">
         <v>8</v>
       </c>
       <c r="G18" s="6"/>
@@ -1983,21 +2148,21 @@
     </row>
     <row r="19" spans="1:22" ht="45.75">
       <c r="A19" s="5" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F19" s="12">
+        <v>55</v>
+      </c>
+      <c r="F19" s="10">
         <v>8</v>
       </c>
       <c r="G19" s="6"/>
@@ -2038,21 +2203,21 @@
     </row>
     <row r="20" spans="1:22" ht="60.75">
       <c r="A20" s="5" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F20" s="12">
+        <v>42</v>
+      </c>
+      <c r="F20" s="10">
         <v>11</v>
       </c>
       <c r="G20" s="6"/>
@@ -2093,7 +2258,7 @@
     </row>
     <row r="21" spans="1:22">
       <c r="A21" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="F21">
         <f>SUM(F6:F20)</f>
@@ -2119,444 +2284,647 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2A67B82-1C1F-433B-A4E4-B4AC96FCB4EE}">
-  <dimension ref="A2:I25"/>
+  <dimension ref="A2:L40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="K5" sqref="K5:K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.28515625" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" customWidth="1"/>
     <col min="5" max="5" width="12.5703125" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" customWidth="1"/>
     <col min="7" max="7" width="12.42578125" customWidth="1"/>
     <col min="8" max="8" width="12.85546875" customWidth="1"/>
+    <col min="11" max="11" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="30" customHeight="1">
-      <c r="A2" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="16" t="s">
+    <row r="2" spans="1:12" ht="30" customHeight="1">
+      <c r="A2" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="C2" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="D2" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="E2" s="13" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="17" t="s">
+      <c r="F2" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="L2" s="21"/>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="K3" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="20"/>
+      <c r="B4" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="K4" s="26" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="17" t="s">
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="K5" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="19"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="K6" s="11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="20"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="17" t="s">
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="20"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="H8" s="13"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="17" t="s">
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="20"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="20"/>
+      <c r="B13" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="H9" s="13"/>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="17" t="s">
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="H14" s="11"/>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="19"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="H15" s="11"/>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="20"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="H16" s="11"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="18" t="s">
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="H17" s="11"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="18" t="s">
+      <c r="B18" s="11"/>
+      <c r="C18" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="20"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="18" t="s">
+      <c r="B20" s="11"/>
+      <c r="C20" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="H13" s="13"/>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="18" t="s">
+      <c r="B21" s="11"/>
+      <c r="C21" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="24"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="18" t="s">
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="H23" s="11"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="18" t="s">
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="24"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="18" t="s">
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="25"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="24"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="18" t="s">
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="14"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="G20" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="H20" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="I20" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="E21" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="F21" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="G21" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="H21" s="13" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="F22" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="G22" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="H22" s="13" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="A23" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="F23" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="G23" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="H23" s="13" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="F24" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="G24" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="H24" s="13" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="F25" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="G25" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="H25" s="13" t="s">
-        <v>109</v>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31" s="26"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="F31" s="26"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="26"/>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="25"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="24"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="12"/>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="H35" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="I35" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="F36" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="G36" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="H36" s="11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="F37" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="G37" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="H37" s="11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="F38" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="H38" s="11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="F39" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="H39" s="11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="H40" s="11" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A12:A13"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Planificacion actualizada y horas calculada correctamente
</commit_message>
<xml_diff>
--- a/Libro.xlsx
+++ b/Libro.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27002"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27021"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{11EF8E83-F8B9-403B-B963-7FA9A05279CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F96CE465-F262-4337-BE68-618BBE814395}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="99">
   <si>
     <t>Participante</t>
   </si>
@@ -50,52 +50,25 @@
     <t>Horas dedicadas a otras actividades</t>
   </si>
   <si>
-    <t>Horas dedicadas por dia</t>
-  </si>
-  <si>
     <t>Horas por iteracion (5 dias)</t>
   </si>
   <si>
+    <t>Horas totales dedicadas al proyecto (7 iteraciones)</t>
+  </si>
+  <si>
     <t>Sergio Horrillo Moreno</t>
   </si>
   <si>
-    <t>Product Owner (20%) : 40'</t>
-  </si>
-  <si>
-    <t>3h20'</t>
-  </si>
-  <si>
-    <t>16h40'</t>
-  </si>
-  <si>
     <t>Guillermo Dueñas Corraliza</t>
   </si>
   <si>
-    <t>SCRUM Master (50%): 3h</t>
-  </si>
-  <si>
-    <t>15h</t>
-  </si>
-  <si>
-    <t>75h</t>
-  </si>
-  <si>
     <t>Ismael Bocadulce Serrano</t>
   </si>
   <si>
-    <t>Desarrollador Senior (100%): 3h</t>
-  </si>
-  <si>
     <t>Javier Rodriguez Mozo</t>
   </si>
   <si>
-    <t>Desarrollador Junior (100%): 90'</t>
-  </si>
-  <si>
-    <t>7h30'</t>
-  </si>
-  <si>
-    <t>37h30'</t>
+    <t>Total:</t>
   </si>
   <si>
     <t>Metodologías ágiles - SCRUM: Lista de tareas de la iteración</t>
@@ -311,154 +284,52 @@
     <t>Leyenda:</t>
   </si>
   <si>
-    <t>PO:  3h</t>
+    <t>PO:</t>
   </si>
   <si>
     <t>PO -&gt; Product Owner</t>
   </si>
   <si>
-    <t>DS: 12h</t>
+    <t>DS:</t>
   </si>
   <si>
     <t>DS -&gt; Desarrollador Senior</t>
   </si>
   <si>
-    <t>PO: 2,6h</t>
+    <t xml:space="preserve">DJ: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SM: </t>
   </si>
   <si>
     <t>DJ -&gt; Desarrollador Junior</t>
   </si>
   <si>
-    <t>SM: 6,5h</t>
-  </si>
-  <si>
     <t>SM -&gt; SCRUM Master</t>
   </si>
   <si>
-    <t>DS: 3,9h</t>
-  </si>
-  <si>
-    <t>DS: 6,3h</t>
-  </si>
-  <si>
-    <t>DJ: 2,7h</t>
-  </si>
-  <si>
-    <t>DJ: 7,5h</t>
-  </si>
-  <si>
-    <t>DS: 7,5h</t>
-  </si>
-  <si>
-    <t>DJ: 5,5h</t>
-  </si>
-  <si>
-    <t>SM: 5,5h</t>
-  </si>
-  <si>
-    <t>PO: 1,6h</t>
-  </si>
-  <si>
-    <t>SM: 4h</t>
-  </si>
-  <si>
-    <t>DS: 2,4h</t>
-  </si>
-  <si>
-    <t>DS: 8h</t>
-  </si>
-  <si>
-    <t>DS: 6,4h</t>
-  </si>
-  <si>
-    <t>DJ: 8h</t>
-  </si>
-  <si>
-    <t>SM: 4,5h</t>
-  </si>
-  <si>
-    <t>DS: 4,5h</t>
-  </si>
-  <si>
-    <t>DS: 9h</t>
-  </si>
-  <si>
-    <t>DJ: 15h</t>
-  </si>
-  <si>
-    <t>PO:1,8h</t>
-  </si>
-  <si>
-    <t>PO: 2,2h</t>
-  </si>
-  <si>
-    <t>SM: 4.4h</t>
-  </si>
-  <si>
-    <t>DS: 4,4h</t>
-  </si>
-  <si>
     <t>Tiempo disponible</t>
   </si>
   <si>
-    <t>40h50'</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>Tiempo utilizado por epico</t>
   </si>
   <si>
-    <t>26h</t>
-  </si>
-  <si>
-    <t>25h</t>
-  </si>
-  <si>
-    <t>22h</t>
-  </si>
-  <si>
-    <t>24h</t>
-  </si>
-  <si>
     <t>Tiempo en reuniones</t>
   </si>
   <si>
-    <t>2h + 2h(Doc)</t>
-  </si>
-  <si>
-    <t>Tiempo productivo</t>
-  </si>
-  <si>
-    <t>32h36'</t>
+    <t>2h+2h(Doc):</t>
+  </si>
+  <si>
+    <t>Tiempo productivo (90%)</t>
   </si>
   <si>
     <t>Tiempo final</t>
   </si>
   <si>
-    <t>30h</t>
-  </si>
-  <si>
-    <t>29h</t>
-  </si>
-  <si>
-    <t>28h</t>
-  </si>
-  <si>
     <t>Tiempo sobrante</t>
-  </si>
-  <si>
-    <t>2h</t>
-  </si>
-  <si>
-    <t>3h</t>
-  </si>
-  <si>
-    <t>6h</t>
-  </si>
-  <si>
-    <t>4h</t>
   </si>
 </sst>
 </file>
@@ -535,7 +406,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -633,6 +504,69 @@
         <color rgb="FF000000"/>
       </right>
       <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -643,8 +577,200 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
       <top/>
       <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thick">
         <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
@@ -653,7 +779,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -683,12 +809,21 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -696,27 +831,48 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -732,6 +888,897 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Horas por iteración</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-BDBE-449C-B02A-26D365154A92}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-BDBE-449C-B02A-26D365154A92}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-BDBE-449C-B02A-26D365154A92}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-BDBE-449C-B02A-26D365154A92}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja1!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Sergio Horrillo Moreno</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Guillermo Dueñas Corraliza</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Ismael Bocadulce Serrano</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Javier Rodriguez Mozo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$F$2:$F$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3FB6-4076-8D16-E2C4E4F75DB4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2124075</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2000250</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Gráfico 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE2DA779-4EF8-71C7-351B-A0207A3DC55F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1031,10 +2078,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1045,10 +2092,10 @@
     <col min="4" max="4" width="25" customWidth="1"/>
     <col min="5" max="5" width="32.140625" customWidth="1"/>
     <col min="6" max="6" width="38.28515625" customWidth="1"/>
-    <col min="7" max="7" width="23.5703125" customWidth="1"/>
+    <col min="7" max="7" width="43.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1071,7 +2118,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1082,50 +2129,50 @@
         <v>10</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E2">
-        <v>7</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" t="s">
+        <f>C2-D2</f>
+        <v>8</v>
+      </c>
+      <c r="F2">
+        <f>PRODUCT(B2,D2)</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="G2">
+        <f>PRODUCT(F2,7)</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>5</v>
       </c>
       <c r="C3">
-        <v>8.5</v>
+        <v>9</v>
       </c>
       <c r="D3">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="E3">
-        <v>6</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <f t="shared" ref="E3:E5" si="0">C3-D3</f>
+        <v>7</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F5" si="1">PRODUCT(B3,D3)</f>
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G5" si="2">PRODUCT(F3,7)</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>5</v>
@@ -1134,24 +2181,24 @@
         <v>9</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E4">
-        <v>6</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B5">
         <v>5</v>
@@ -1160,23 +2207,53 @@
         <v>10</v>
       </c>
       <c r="D5">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="E5">
-        <v>7.5</v>
-      </c>
-      <c r="F5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" t="s">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <f>SUM(B2:B5)</f>
         <v>20</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ref="C7:G7" si="3">SUM(C2:C5)</f>
+        <v>38</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="3"/>
+        <v>280</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1184,7 +2261,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EFCC409-402D-4C04-8FD5-6A2AF15AE81D}">
   <dimension ref="A1:V26"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
@@ -1196,7 +2273,7 @@
   <sheetData>
     <row r="1" spans="1:22" ht="28.5">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1222,7 +2299,7 @@
     </row>
     <row r="2" spans="1:22" ht="28.5">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1253,116 +2330,116 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="17"/>
-      <c r="I3" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" s="17"/>
-      <c r="K3" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" s="17"/>
-      <c r="M3" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="N3" s="17"/>
-      <c r="O3" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="R3" s="17"/>
-      <c r="S3" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="T3" s="17"/>
+      <c r="G3" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="28"/>
+      <c r="I3" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="28"/>
+      <c r="K3" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" s="28"/>
+      <c r="M3" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="N3" s="28"/>
+      <c r="O3" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="P3" s="28"/>
+      <c r="Q3" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="R3" s="28"/>
+      <c r="S3" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="T3" s="28"/>
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
     </row>
     <row r="4" spans="1:22" ht="60.75">
       <c r="A4" s="3" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="S4" s="4" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="T4" s="4" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="U4" s="2"/>
       <c r="V4" s="2"/>
     </row>
     <row r="5" spans="1:22" ht="45.75">
       <c r="A5" s="5" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="F5" s="10">
         <v>15</v>
@@ -1407,19 +2484,19 @@
     </row>
     <row r="6" spans="1:22" ht="45.75">
       <c r="A6" s="5" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="F6" s="10">
         <v>13</v>
@@ -1464,19 +2541,19 @@
     </row>
     <row r="7" spans="1:22" ht="60.75">
       <c r="A7" s="5" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="F7" s="10">
         <v>9</v>
@@ -1521,19 +2598,19 @@
     </row>
     <row r="8" spans="1:22" ht="91.5">
       <c r="A8" s="5" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="F8" s="10">
         <v>15</v>
@@ -1578,19 +2655,19 @@
     </row>
     <row r="9" spans="1:22" ht="60.75">
       <c r="A9" s="5" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="F9" s="10">
         <v>11</v>
@@ -1635,19 +2712,19 @@
     </row>
     <row r="10" spans="1:22" ht="45.75">
       <c r="A10" s="5" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="F10" s="10">
         <v>8</v>
@@ -1692,19 +2769,19 @@
     </row>
     <row r="11" spans="1:22" ht="45.75">
       <c r="A11" s="5" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="F11" s="10">
         <v>8</v>
@@ -1749,19 +2826,19 @@
     </row>
     <row r="12" spans="1:22" ht="60.75">
       <c r="A12" s="5" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="F12" s="10">
         <v>8</v>
@@ -1806,19 +2883,19 @@
     </row>
     <row r="13" spans="1:22" ht="60.75">
       <c r="A13" s="5" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="F13" s="10">
         <v>8</v>
@@ -1863,19 +2940,19 @@
     </row>
     <row r="14" spans="1:22" ht="60.75">
       <c r="A14" s="5" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="F14" s="10">
         <v>9</v>
@@ -1920,19 +2997,19 @@
     </row>
     <row r="15" spans="1:22" ht="76.5">
       <c r="A15" s="5" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="F15" s="10">
         <v>8</v>
@@ -1977,19 +3054,19 @@
     </row>
     <row r="16" spans="1:22" s="8" customFormat="1" ht="57.75" customHeight="1">
       <c r="A16" s="5" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="F16" s="10">
         <v>24</v>
@@ -2034,19 +3111,19 @@
     </row>
     <row r="17" spans="1:22" ht="76.5">
       <c r="A17" s="5" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="F17" s="10">
         <v>9</v>
@@ -2091,19 +3168,19 @@
     </row>
     <row r="18" spans="1:22" ht="45.75">
       <c r="A18" s="5" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="F18" s="10">
         <v>8</v>
@@ -2148,19 +3225,19 @@
     </row>
     <row r="19" spans="1:22" ht="45.75">
       <c r="A19" s="5" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="F19" s="10">
         <v>8</v>
@@ -2203,19 +3280,19 @@
     </row>
     <row r="20" spans="1:22" ht="60.75">
       <c r="A20" s="5" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="F20" s="10">
         <v>11</v>
@@ -2258,7 +3335,7 @@
     </row>
     <row r="21" spans="1:22">
       <c r="A21" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="F21">
         <f>SUM(F6:F20)</f>
@@ -2284,646 +3361,1760 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2A67B82-1C1F-433B-A4E4-B4AC96FCB4EE}">
-  <dimension ref="A2:L40"/>
+  <dimension ref="A2:R74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5:K6"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="R49" sqref="R49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="3.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="3.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="3.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" customWidth="1"/>
+    <col min="9" max="9" width="3.7109375" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" customWidth="1"/>
+    <col min="11" max="11" width="3.7109375" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" customWidth="1"/>
+    <col min="13" max="13" width="3.7109375" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" customWidth="1"/>
+    <col min="15" max="15" width="3.7109375" customWidth="1"/>
+    <col min="18" max="18" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" ht="30" customHeight="1">
-      <c r="A2" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" s="13" t="s">
+    <row r="2" spans="1:18" ht="30" customHeight="1">
+      <c r="A2" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="42"/>
+      <c r="D2" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="42"/>
+      <c r="F2" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="42"/>
+      <c r="H2" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="42"/>
+      <c r="J2" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="42"/>
+      <c r="L2" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="42"/>
+      <c r="N2" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="39"/>
+      <c r="R2" s="13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="22" t="s">
-        <v>91</v>
-      </c>
-      <c r="L2" s="21"/>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="K3" s="11" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" s="20"/>
+      <c r="B3" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="15">
+        <v>4</v>
+      </c>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="25"/>
+      <c r="R3" s="11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" s="31"/>
       <c r="B4" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="C4" s="11"/>
+        <v>85</v>
+      </c>
+      <c r="C4" s="11">
+        <v>4</v>
+      </c>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
-      <c r="K4" s="26" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="19"/>
+      <c r="R4" s="14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" s="31"/>
+      <c r="B5" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="11">
+        <v>4</v>
+      </c>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
-      <c r="F5" s="11" t="s">
-        <v>96</v>
-      </c>
+      <c r="F5" s="11"/>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
-      <c r="K5" s="11" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="19"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="K6" s="11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="20"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="18" t="s">
-        <v>46</v>
-      </c>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="19"/>
+      <c r="R5" s="14"/>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" s="31"/>
+      <c r="B6" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="14">
+        <v>3</v>
+      </c>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="22"/>
+      <c r="R6" s="14"/>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="K7" s="17">
+        <v>3</v>
+      </c>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="18"/>
+      <c r="R7" s="11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" s="31"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
-      <c r="F8" s="11" t="s">
-        <v>101</v>
-      </c>
+      <c r="F8" s="11"/>
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="20"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="K8" s="11">
+        <v>3</v>
+      </c>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="19"/>
+      <c r="R8" s="11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" s="31"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
-      <c r="F9" s="11" t="s">
-        <v>102</v>
-      </c>
+      <c r="F9" s="11"/>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="20"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>105</v>
-      </c>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="K9" s="11">
+        <v>3</v>
+      </c>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="19"/>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10" s="31"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="K10" s="14">
+        <v>4</v>
+      </c>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="22"/>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="K11" s="17">
+        <v>2</v>
+      </c>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="17"/>
+      <c r="O11" s="18"/>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="A12" s="31"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="20"/>
-      <c r="B13" s="11" t="s">
-        <v>106</v>
-      </c>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="K12" s="11">
+        <v>2</v>
+      </c>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="19"/>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13" s="31"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="H14" s="11"/>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="19"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="H15" s="11"/>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="A16" s="20"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="K13" s="11">
+        <v>3</v>
+      </c>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="19"/>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" s="31"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="K14" s="14">
+        <v>2</v>
+      </c>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="22"/>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="I15" s="17">
+        <v>4</v>
+      </c>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="18"/>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="A16" s="31"/>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
-      <c r="G16" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="H16" s="11"/>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="14" t="s">
-        <v>59</v>
-      </c>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="I16" s="11">
+        <v>3</v>
+      </c>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="19"/>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="A17" s="31"/>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
-      <c r="G17" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="H17" s="11"/>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="20"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11" t="s">
-        <v>112</v>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="I17" s="11">
+        <v>4</v>
+      </c>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="19"/>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18" s="31"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="I18" s="14">
+        <v>4</v>
+      </c>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="22"/>
+    </row>
+    <row r="19" spans="1:15">
+      <c r="A19" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" s="17">
+        <v>2</v>
+      </c>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="17"/>
+      <c r="O19" s="18"/>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" s="31"/>
+      <c r="B20" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="11">
+        <v>3</v>
       </c>
       <c r="D20" s="11"/>
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
       <c r="H20" s="11"/>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11" t="s">
-        <v>113</v>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="19"/>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21" s="31"/>
+      <c r="B21" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="C21" s="11">
+        <v>3</v>
       </c>
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="24"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="H23" s="11"/>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="23" t="s">
-        <v>74</v>
-      </c>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="19"/>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22" s="31"/>
+      <c r="B22" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" s="14">
+        <v>3</v>
+      </c>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="14"/>
+      <c r="O22" s="22"/>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="A23" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="17"/>
+      <c r="L23" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="M23" s="17">
+        <v>2</v>
+      </c>
+      <c r="N23" s="17"/>
+      <c r="O23" s="18"/>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24" s="31"/>
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
       <c r="D24" s="11"/>
       <c r="E24" s="11"/>
       <c r="F24" s="11"/>
       <c r="G24" s="11"/>
-      <c r="H24" s="11" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="24"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="M24" s="11">
+        <v>2</v>
+      </c>
+      <c r="N24" s="11"/>
+      <c r="O24" s="19"/>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25" s="31"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
       <c r="D25" s="11"/>
       <c r="E25" s="11"/>
       <c r="F25" s="11"/>
       <c r="G25" s="11"/>
-      <c r="H25" s="11" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="25"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="24"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="M25" s="11">
+        <v>2</v>
+      </c>
+      <c r="N25" s="11"/>
+      <c r="O25" s="19"/>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="A26" s="31"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="14"/>
+      <c r="L26" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="M26" s="14">
+        <v>2</v>
+      </c>
+      <c r="N26" s="14"/>
+      <c r="O26" s="22"/>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="A27" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="17"/>
+      <c r="L27" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="M27" s="17">
+        <v>2</v>
+      </c>
+      <c r="N27" s="17"/>
+      <c r="O27" s="18"/>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="A28" s="31"/>
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
-      <c r="D28" s="11" t="s">
-        <v>102</v>
-      </c>
+      <c r="D28" s="11"/>
       <c r="E28" s="11"/>
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
       <c r="H28" s="11"/>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="15" t="s">
-        <v>80</v>
-      </c>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="M28" s="11">
+        <v>2</v>
+      </c>
+      <c r="N28" s="11"/>
+      <c r="O28" s="19"/>
+    </row>
+    <row r="29" spans="1:15">
+      <c r="A29" s="31"/>
       <c r="B29" s="11"/>
       <c r="C29" s="11"/>
-      <c r="D29" s="11" t="s">
-        <v>110</v>
-      </c>
+      <c r="D29" s="11"/>
       <c r="E29" s="11"/>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
       <c r="H29" s="11"/>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="15" t="s">
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="M29" s="11">
+        <v>2</v>
+      </c>
+      <c r="N29" s="11"/>
+      <c r="O29" s="19"/>
+    </row>
+    <row r="30" spans="1:15">
+      <c r="A30" s="31"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="14"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="M30" s="14">
+        <v>2</v>
+      </c>
+      <c r="N30" s="14"/>
+      <c r="O30" s="22"/>
+    </row>
+    <row r="31" spans="1:15">
+      <c r="A31" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="B31" s="26"/>
-      <c r="C31" s="26"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="26" t="s">
-        <v>118</v>
-      </c>
-      <c r="F31" s="26"/>
-      <c r="G31" s="26"/>
-      <c r="H31" s="26"/>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="A32" s="25"/>
+      <c r="E31" s="17">
+        <v>2</v>
+      </c>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="17"/>
+      <c r="J31" s="17"/>
+      <c r="K31" s="17"/>
+      <c r="L31" s="17"/>
+      <c r="M31" s="17"/>
+      <c r="N31" s="17"/>
+      <c r="O31" s="18"/>
+    </row>
+    <row r="32" spans="1:15">
+      <c r="A32" s="31"/>
       <c r="B32" s="11"/>
       <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11" t="s">
-        <v>119</v>
+      <c r="D32" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E32" s="11">
+        <v>2</v>
       </c>
       <c r="F32" s="11"/>
       <c r="G32" s="11"/>
       <c r="H32" s="11"/>
-    </row>
-    <row r="33" spans="1:9">
-      <c r="A33" s="24"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="11"/>
+      <c r="M32" s="11"/>
+      <c r="N32" s="11"/>
+      <c r="O32" s="19"/>
+    </row>
+    <row r="33" spans="1:15">
+      <c r="A33" s="31"/>
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11" t="s">
-        <v>120</v>
+      <c r="D33" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="E33" s="11">
+        <v>2</v>
       </c>
       <c r="F33" s="11"/>
       <c r="G33" s="11"/>
       <c r="H33" s="11"/>
-    </row>
-    <row r="34" spans="1:9">
-      <c r="A34" s="12"/>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="A35" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="B35" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="E35" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="F35" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="G35" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="H35" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="I35" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9">
-      <c r="A36" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="B36" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>126</v>
-      </c>
+      <c r="I33" s="11"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="11"/>
+      <c r="L33" s="11"/>
+      <c r="M33" s="11"/>
+      <c r="N33" s="11"/>
+      <c r="O33" s="19"/>
+    </row>
+    <row r="34" spans="1:15">
+      <c r="A34" s="31"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="E34" s="14">
+        <v>2</v>
+      </c>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="14"/>
+      <c r="J34" s="14"/>
+      <c r="K34" s="14"/>
+      <c r="L34" s="14"/>
+      <c r="M34" s="14"/>
+      <c r="N34" s="14"/>
+      <c r="O34" s="22"/>
+    </row>
+    <row r="35" spans="1:15">
+      <c r="A35" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" s="17"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="E35" s="17">
+        <v>2</v>
+      </c>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="17"/>
+      <c r="J35" s="17"/>
+      <c r="K35" s="17"/>
+      <c r="L35" s="17"/>
+      <c r="M35" s="17"/>
+      <c r="N35" s="17"/>
+      <c r="O35" s="18"/>
+    </row>
+    <row r="36" spans="1:15">
+      <c r="A36" s="34"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
       <c r="D36" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="E36" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="F36" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="G36" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="H36" s="11" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
-      <c r="A37" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="B37" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="C37" s="11" t="s">
-        <v>130</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="E36" s="11">
+        <v>2</v>
+      </c>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="11"/>
+      <c r="J36" s="11"/>
+      <c r="K36" s="11"/>
+      <c r="L36" s="11"/>
+      <c r="M36" s="11"/>
+      <c r="N36" s="11"/>
+      <c r="O36" s="19"/>
+    </row>
+    <row r="37" spans="1:15">
+      <c r="A37" s="34"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
       <c r="D37" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="E37" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="F37" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="G37" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="H37" s="11" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
-      <c r="A38" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="B38" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="C38" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="E38" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="F38" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="G38" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="H38" s="11" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9">
-      <c r="A39" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="B39" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="E39" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="F39" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="G39" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="H39" s="11" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9">
-      <c r="A40" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="B40" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>139</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="E37" s="11">
+        <v>2</v>
+      </c>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="11"/>
+      <c r="J37" s="11"/>
+      <c r="K37" s="11"/>
+      <c r="L37" s="11"/>
+      <c r="M37" s="11"/>
+      <c r="N37" s="11"/>
+      <c r="O37" s="19"/>
+    </row>
+    <row r="38" spans="1:15">
+      <c r="A38" s="34"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="E38" s="14">
+        <v>2</v>
+      </c>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="14"/>
+      <c r="J38" s="14"/>
+      <c r="K38" s="14"/>
+      <c r="L38" s="14"/>
+      <c r="M38" s="14"/>
+      <c r="N38" s="14"/>
+      <c r="O38" s="22"/>
+    </row>
+    <row r="39" spans="1:15">
+      <c r="A39" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="E39" s="17">
+        <v>2</v>
+      </c>
+      <c r="F39" s="17"/>
+      <c r="G39" s="17"/>
+      <c r="H39" s="17"/>
+      <c r="I39" s="17"/>
+      <c r="J39" s="17"/>
+      <c r="K39" s="17"/>
+      <c r="L39" s="17"/>
+      <c r="M39" s="17"/>
+      <c r="N39" s="17"/>
+      <c r="O39" s="18"/>
+    </row>
+    <row r="40" spans="1:15">
+      <c r="A40" s="34"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
       <c r="D40" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="E40" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="F40" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="G40" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="H40" s="11" t="s">
-        <v>141</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="E40" s="11">
+        <v>2</v>
+      </c>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="11"/>
+      <c r="J40" s="11"/>
+      <c r="K40" s="11"/>
+      <c r="L40" s="11"/>
+      <c r="M40" s="11"/>
+      <c r="N40" s="11"/>
+      <c r="O40" s="19"/>
+    </row>
+    <row r="41" spans="1:15">
+      <c r="A41" s="34"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="E41" s="11">
+        <v>2</v>
+      </c>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="11"/>
+      <c r="J41" s="11"/>
+      <c r="K41" s="11"/>
+      <c r="L41" s="11"/>
+      <c r="M41" s="11"/>
+      <c r="N41" s="11"/>
+      <c r="O41" s="19"/>
+    </row>
+    <row r="42" spans="1:15">
+      <c r="A42" s="34"/>
+      <c r="B42" s="14"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="E42" s="14">
+        <v>3</v>
+      </c>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="14"/>
+      <c r="K42" s="14"/>
+      <c r="L42" s="14"/>
+      <c r="M42" s="14"/>
+      <c r="N42" s="14"/>
+      <c r="O42" s="22"/>
+    </row>
+    <row r="43" spans="1:15">
+      <c r="A43" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="B43" s="17"/>
+      <c r="C43" s="17"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="17"/>
+      <c r="H43" s="17"/>
+      <c r="I43" s="17"/>
+      <c r="J43" s="17"/>
+      <c r="K43" s="17"/>
+      <c r="L43" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="M43" s="17">
+        <v>2</v>
+      </c>
+      <c r="N43" s="17"/>
+      <c r="O43" s="18"/>
+    </row>
+    <row r="44" spans="1:15">
+      <c r="A44" s="34"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="11"/>
+      <c r="J44" s="11"/>
+      <c r="K44" s="11"/>
+      <c r="L44" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="M44" s="11">
+        <v>2</v>
+      </c>
+      <c r="N44" s="11"/>
+      <c r="O44" s="19"/>
+    </row>
+    <row r="45" spans="1:15">
+      <c r="A45" s="34"/>
+      <c r="B45" s="11"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="11"/>
+      <c r="J45" s="11"/>
+      <c r="K45" s="11"/>
+      <c r="L45" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="M45" s="11">
+        <v>2</v>
+      </c>
+      <c r="N45" s="11"/>
+      <c r="O45" s="19"/>
+    </row>
+    <row r="46" spans="1:15">
+      <c r="A46" s="34"/>
+      <c r="B46" s="14"/>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="14"/>
+      <c r="G46" s="14"/>
+      <c r="H46" s="14"/>
+      <c r="I46" s="14"/>
+      <c r="J46" s="14"/>
+      <c r="K46" s="14"/>
+      <c r="L46" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="M46" s="14">
+        <v>2</v>
+      </c>
+      <c r="N46" s="14"/>
+      <c r="O46" s="22"/>
+    </row>
+    <row r="47" spans="1:15">
+      <c r="A47" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="B47" s="17"/>
+      <c r="C47" s="17"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="17"/>
+      <c r="H47" s="17"/>
+      <c r="I47" s="17"/>
+      <c r="J47" s="17"/>
+      <c r="K47" s="17"/>
+      <c r="L47" s="17"/>
+      <c r="M47" s="17"/>
+      <c r="N47" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="O47" s="18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15">
+      <c r="A48" s="34"/>
+      <c r="B48" s="11"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
+      <c r="I48" s="11"/>
+      <c r="J48" s="11"/>
+      <c r="K48" s="11"/>
+      <c r="L48" s="11"/>
+      <c r="M48" s="11"/>
+      <c r="N48" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="O48" s="19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15">
+      <c r="A49" s="34"/>
+      <c r="B49" s="11"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="11"/>
+      <c r="G49" s="11"/>
+      <c r="H49" s="11"/>
+      <c r="I49" s="11"/>
+      <c r="J49" s="11"/>
+      <c r="K49" s="11"/>
+      <c r="L49" s="11"/>
+      <c r="M49" s="11"/>
+      <c r="N49" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="O49" s="19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15">
+      <c r="A50" s="35"/>
+      <c r="B50" s="20"/>
+      <c r="C50" s="20"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="20"/>
+      <c r="F50" s="20"/>
+      <c r="G50" s="20"/>
+      <c r="H50" s="20"/>
+      <c r="I50" s="20"/>
+      <c r="J50" s="20"/>
+      <c r="K50" s="20"/>
+      <c r="L50" s="20"/>
+      <c r="M50" s="20"/>
+      <c r="N50" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="O50" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15">
+      <c r="A51" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="B51" s="15"/>
+      <c r="C51" s="15"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="15"/>
+      <c r="F51" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="G51" s="15">
+        <v>3</v>
+      </c>
+      <c r="H51" s="15"/>
+      <c r="I51" s="15"/>
+      <c r="J51" s="15"/>
+      <c r="K51" s="15"/>
+      <c r="L51" s="15"/>
+      <c r="M51" s="15"/>
+      <c r="N51" s="15"/>
+      <c r="O51" s="25"/>
+    </row>
+    <row r="52" spans="1:15">
+      <c r="A52" s="34"/>
+      <c r="B52" s="11"/>
+      <c r="C52" s="11"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="11"/>
+      <c r="F52" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="G52" s="11">
+        <v>2</v>
+      </c>
+      <c r="H52" s="11"/>
+      <c r="I52" s="11"/>
+      <c r="J52" s="11"/>
+      <c r="K52" s="11"/>
+      <c r="L52" s="11"/>
+      <c r="M52" s="11"/>
+      <c r="N52" s="11"/>
+      <c r="O52" s="19"/>
+    </row>
+    <row r="53" spans="1:15">
+      <c r="A53" s="34"/>
+      <c r="B53" s="11"/>
+      <c r="C53" s="11"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="11"/>
+      <c r="F53" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="G53" s="11">
+        <v>2</v>
+      </c>
+      <c r="H53" s="11"/>
+      <c r="I53" s="11"/>
+      <c r="J53" s="11"/>
+      <c r="K53" s="11"/>
+      <c r="L53" s="11"/>
+      <c r="M53" s="11"/>
+      <c r="N53" s="11"/>
+      <c r="O53" s="19"/>
+    </row>
+    <row r="54" spans="1:15">
+      <c r="A54" s="34"/>
+      <c r="B54" s="14"/>
+      <c r="C54" s="14"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="G54" s="14">
+        <v>2</v>
+      </c>
+      <c r="H54" s="14"/>
+      <c r="I54" s="14"/>
+      <c r="J54" s="14"/>
+      <c r="K54" s="14"/>
+      <c r="L54" s="14"/>
+      <c r="M54" s="14"/>
+      <c r="N54" s="14"/>
+      <c r="O54" s="22"/>
+    </row>
+    <row r="55" spans="1:15">
+      <c r="A55" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="B55" s="17"/>
+      <c r="C55" s="17"/>
+      <c r="D55" s="17"/>
+      <c r="E55" s="17"/>
+      <c r="F55" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="G55" s="17">
+        <v>2</v>
+      </c>
+      <c r="H55" s="17"/>
+      <c r="I55" s="17"/>
+      <c r="J55" s="17"/>
+      <c r="K55" s="17"/>
+      <c r="L55" s="17"/>
+      <c r="M55" s="17"/>
+      <c r="N55" s="17"/>
+      <c r="O55" s="18"/>
+    </row>
+    <row r="56" spans="1:15">
+      <c r="A56" s="34"/>
+      <c r="B56" s="11"/>
+      <c r="C56" s="11"/>
+      <c r="D56" s="11"/>
+      <c r="E56" s="11"/>
+      <c r="F56" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="G56" s="11">
+        <v>2</v>
+      </c>
+      <c r="H56" s="11"/>
+      <c r="I56" s="11"/>
+      <c r="J56" s="11"/>
+      <c r="K56" s="11"/>
+      <c r="L56" s="11"/>
+      <c r="M56" s="11"/>
+      <c r="N56" s="11"/>
+      <c r="O56" s="19"/>
+    </row>
+    <row r="57" spans="1:15">
+      <c r="A57" s="34"/>
+      <c r="B57" s="11"/>
+      <c r="C57" s="11"/>
+      <c r="D57" s="11"/>
+      <c r="E57" s="11"/>
+      <c r="F57" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="G57" s="11">
+        <v>2</v>
+      </c>
+      <c r="H57" s="11"/>
+      <c r="I57" s="11"/>
+      <c r="J57" s="11"/>
+      <c r="K57" s="11"/>
+      <c r="L57" s="11"/>
+      <c r="M57" s="11"/>
+      <c r="N57" s="11"/>
+      <c r="O57" s="19"/>
+    </row>
+    <row r="58" spans="1:15">
+      <c r="A58" s="34"/>
+      <c r="B58" s="14"/>
+      <c r="C58" s="14"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="G58" s="14">
+        <v>2</v>
+      </c>
+      <c r="H58" s="14"/>
+      <c r="I58" s="14"/>
+      <c r="J58" s="14"/>
+      <c r="K58" s="14"/>
+      <c r="L58" s="14"/>
+      <c r="M58" s="14"/>
+      <c r="N58" s="14"/>
+      <c r="O58" s="22"/>
+    </row>
+    <row r="59" spans="1:15">
+      <c r="A59" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="B59" s="17"/>
+      <c r="C59" s="17"/>
+      <c r="D59" s="17"/>
+      <c r="E59" s="17"/>
+      <c r="F59" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="G59" s="17">
+        <v>2</v>
+      </c>
+      <c r="H59" s="17"/>
+      <c r="I59" s="17"/>
+      <c r="J59" s="17"/>
+      <c r="K59" s="17"/>
+      <c r="L59" s="17"/>
+      <c r="M59" s="17"/>
+      <c r="N59" s="17"/>
+      <c r="O59" s="18"/>
+    </row>
+    <row r="60" spans="1:15">
+      <c r="A60" s="34"/>
+      <c r="B60" s="14"/>
+      <c r="C60" s="14"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="14"/>
+      <c r="F60" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="G60" s="11">
+        <v>2</v>
+      </c>
+      <c r="H60" s="14"/>
+      <c r="I60" s="14"/>
+      <c r="J60" s="14"/>
+      <c r="K60" s="14"/>
+      <c r="L60" s="14"/>
+      <c r="M60" s="14"/>
+      <c r="N60" s="14"/>
+      <c r="O60" s="22"/>
+    </row>
+    <row r="61" spans="1:15">
+      <c r="A61" s="34"/>
+      <c r="B61" s="14"/>
+      <c r="C61" s="14"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="14"/>
+      <c r="F61" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="G61" s="11">
+        <v>2</v>
+      </c>
+      <c r="H61" s="14"/>
+      <c r="I61" s="14"/>
+      <c r="J61" s="14"/>
+      <c r="K61" s="14"/>
+      <c r="L61" s="14"/>
+      <c r="M61" s="14"/>
+      <c r="N61" s="14"/>
+      <c r="O61" s="22"/>
+    </row>
+    <row r="62" spans="1:15">
+      <c r="A62" s="34"/>
+      <c r="B62" s="14"/>
+      <c r="C62" s="14"/>
+      <c r="D62" s="14"/>
+      <c r="E62" s="14"/>
+      <c r="F62" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="G62" s="14">
+        <v>2</v>
+      </c>
+      <c r="H62" s="14"/>
+      <c r="I62" s="14"/>
+      <c r="J62" s="14"/>
+      <c r="K62" s="14"/>
+      <c r="L62" s="14"/>
+      <c r="M62" s="14"/>
+      <c r="N62" s="14"/>
+      <c r="O62" s="22"/>
+    </row>
+    <row r="63" spans="1:15">
+      <c r="A63" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="B63" s="23"/>
+      <c r="C63" s="23"/>
+      <c r="D63" s="23"/>
+      <c r="E63" s="23"/>
+      <c r="F63" s="23"/>
+      <c r="G63" s="23"/>
+      <c r="H63" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="I63" s="17">
+        <v>3</v>
+      </c>
+      <c r="J63" s="23"/>
+      <c r="K63" s="23"/>
+      <c r="L63" s="23"/>
+      <c r="M63" s="23"/>
+      <c r="N63" s="23"/>
+      <c r="O63" s="24"/>
+    </row>
+    <row r="64" spans="1:15">
+      <c r="A64" s="34"/>
+      <c r="B64" s="14"/>
+      <c r="C64" s="14"/>
+      <c r="D64" s="14"/>
+      <c r="E64" s="14"/>
+      <c r="F64" s="14"/>
+      <c r="G64" s="14"/>
+      <c r="H64" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="I64" s="11">
+        <v>2</v>
+      </c>
+      <c r="J64" s="14"/>
+      <c r="K64" s="14"/>
+      <c r="L64" s="14"/>
+      <c r="M64" s="14"/>
+      <c r="N64" s="14"/>
+      <c r="O64" s="22"/>
+    </row>
+    <row r="65" spans="1:16">
+      <c r="A65" s="34"/>
+      <c r="B65" s="11"/>
+      <c r="C65" s="11"/>
+      <c r="D65" s="11"/>
+      <c r="E65" s="11"/>
+      <c r="F65" s="11"/>
+      <c r="G65" s="11"/>
+      <c r="H65" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="I65" s="11">
+        <v>3</v>
+      </c>
+      <c r="J65" s="11"/>
+      <c r="K65" s="11"/>
+      <c r="L65" s="11"/>
+      <c r="M65" s="11"/>
+      <c r="N65" s="11"/>
+      <c r="O65" s="19"/>
+    </row>
+    <row r="66" spans="1:16">
+      <c r="A66" s="35"/>
+      <c r="B66" s="20"/>
+      <c r="C66" s="20"/>
+      <c r="D66" s="20"/>
+      <c r="E66" s="20"/>
+      <c r="F66" s="20"/>
+      <c r="G66" s="20"/>
+      <c r="H66" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="I66" s="20">
+        <v>3</v>
+      </c>
+      <c r="J66" s="20"/>
+      <c r="K66" s="20"/>
+      <c r="L66" s="20"/>
+      <c r="M66" s="20"/>
+      <c r="N66" s="20"/>
+      <c r="O66" s="21"/>
+    </row>
+    <row r="67" spans="1:16">
+      <c r="A67" s="12"/>
+    </row>
+    <row r="68" spans="1:16">
+      <c r="A68" s="12"/>
+    </row>
+    <row r="69" spans="1:16">
+      <c r="A69" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B69" s="37">
+        <v>35</v>
+      </c>
+      <c r="C69" s="37"/>
+      <c r="D69" s="37">
+        <v>35</v>
+      </c>
+      <c r="E69" s="37"/>
+      <c r="F69" s="37">
+        <v>35</v>
+      </c>
+      <c r="G69" s="37"/>
+      <c r="H69" s="37">
+        <v>35</v>
+      </c>
+      <c r="I69" s="37"/>
+      <c r="J69" s="37">
+        <v>35</v>
+      </c>
+      <c r="K69" s="37"/>
+      <c r="L69" s="37">
+        <v>35</v>
+      </c>
+      <c r="M69" s="37"/>
+      <c r="N69" s="37">
+        <v>35</v>
+      </c>
+      <c r="O69" s="37"/>
+      <c r="P69" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16">
+      <c r="A70" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="B70" s="40">
+        <f>SUM(C3:C66)</f>
+        <v>26</v>
+      </c>
+      <c r="C70" s="41"/>
+      <c r="D70" s="36">
+        <f>SUM(E3:E66)</f>
+        <v>25</v>
+      </c>
+      <c r="E70" s="36"/>
+      <c r="F70" s="36">
+        <f>SUM(G3:G66)</f>
+        <v>25</v>
+      </c>
+      <c r="G70" s="36"/>
+      <c r="H70" s="36">
+        <f>SUM(I3:I66)</f>
+        <v>26</v>
+      </c>
+      <c r="I70" s="36"/>
+      <c r="J70" s="36">
+        <f>SUM(K3:K66)</f>
+        <v>22</v>
+      </c>
+      <c r="K70" s="36"/>
+      <c r="L70" s="36">
+        <f>SUM(M3:M66)</f>
+        <v>24</v>
+      </c>
+      <c r="M70" s="36"/>
+      <c r="N70" s="36">
+        <f>SUM(O3:O66)</f>
+        <v>24</v>
+      </c>
+      <c r="O70" s="36"/>
+    </row>
+    <row r="71" spans="1:16">
+      <c r="A71" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B71" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C71" s="11">
+        <v>4</v>
+      </c>
+      <c r="D71" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E71" s="11">
+        <v>4</v>
+      </c>
+      <c r="F71" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="G71" s="11">
+        <v>4</v>
+      </c>
+      <c r="H71" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="I71" s="11">
+        <v>4</v>
+      </c>
+      <c r="J71" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="K71" s="11">
+        <v>4</v>
+      </c>
+      <c r="L71" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="M71" s="11">
+        <v>4</v>
+      </c>
+      <c r="N71" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="O71" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16">
+      <c r="A72" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B72" s="29">
+        <v>31.5</v>
+      </c>
+      <c r="C72" s="30"/>
+      <c r="D72" s="29">
+        <v>31.5</v>
+      </c>
+      <c r="E72" s="30"/>
+      <c r="F72" s="29">
+        <v>31.5</v>
+      </c>
+      <c r="G72" s="30"/>
+      <c r="H72" s="29">
+        <v>31.5</v>
+      </c>
+      <c r="I72" s="30"/>
+      <c r="J72" s="29">
+        <v>31.5</v>
+      </c>
+      <c r="K72" s="30"/>
+      <c r="L72" s="29">
+        <v>31.5</v>
+      </c>
+      <c r="M72" s="30"/>
+      <c r="N72" s="29">
+        <v>31.5</v>
+      </c>
+      <c r="O72" s="30"/>
+    </row>
+    <row r="73" spans="1:16">
+      <c r="A73" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="B73" s="29">
+        <f>SUM(B70,C71)</f>
+        <v>30</v>
+      </c>
+      <c r="C73" s="30"/>
+      <c r="D73" s="29">
+        <f t="shared" ref="D73:O73" si="0">SUM(D70,E71)</f>
+        <v>29</v>
+      </c>
+      <c r="E73" s="30"/>
+      <c r="F73" s="29">
+        <f t="shared" ref="F73:O73" si="1">SUM(F70,G71)</f>
+        <v>29</v>
+      </c>
+      <c r="G73" s="30"/>
+      <c r="H73" s="29">
+        <f t="shared" ref="H73:O73" si="2">SUM(H70,I71)</f>
+        <v>30</v>
+      </c>
+      <c r="I73" s="30"/>
+      <c r="J73" s="29">
+        <f t="shared" ref="J73:O73" si="3">SUM(J70,K71)</f>
+        <v>26</v>
+      </c>
+      <c r="K73" s="30"/>
+      <c r="L73" s="29">
+        <f t="shared" ref="L73:O73" si="4">SUM(L70,M71)</f>
+        <v>28</v>
+      </c>
+      <c r="M73" s="30"/>
+      <c r="N73" s="29">
+        <f t="shared" ref="N73:O73" si="5">SUM(N70,O71)</f>
+        <v>28</v>
+      </c>
+      <c r="O73" s="30"/>
+    </row>
+    <row r="74" spans="1:16">
+      <c r="A74" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B74" s="29">
+        <f>B72-B73</f>
+        <v>1.5</v>
+      </c>
+      <c r="C74" s="30"/>
+      <c r="D74" s="29">
+        <f t="shared" ref="D74" si="6">D72-D73</f>
+        <v>2.5</v>
+      </c>
+      <c r="E74" s="30"/>
+      <c r="F74" s="29">
+        <f t="shared" ref="F74" si="7">F72-F73</f>
+        <v>2.5</v>
+      </c>
+      <c r="G74" s="30"/>
+      <c r="H74" s="29">
+        <f t="shared" ref="H74" si="8">H72-H73</f>
+        <v>1.5</v>
+      </c>
+      <c r="I74" s="30"/>
+      <c r="J74" s="29">
+        <f t="shared" ref="J74" si="9">J72-J73</f>
+        <v>5.5</v>
+      </c>
+      <c r="K74" s="30"/>
+      <c r="L74" s="29">
+        <f t="shared" ref="L74" si="10">L72-L73</f>
+        <v>3.5</v>
+      </c>
+      <c r="M74" s="30"/>
+      <c r="N74" s="29">
+        <f t="shared" ref="N74" si="11">N72-N73</f>
+        <v>3.5</v>
+      </c>
+      <c r="O74" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A12:A13"/>
+  <mergeCells count="58">
+    <mergeCell ref="A51:A54"/>
+    <mergeCell ref="A55:A58"/>
+    <mergeCell ref="A59:A62"/>
+    <mergeCell ref="A63:A66"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="F70:G70"/>
+    <mergeCell ref="F69:G69"/>
+    <mergeCell ref="J70:K70"/>
+    <mergeCell ref="J69:K69"/>
+    <mergeCell ref="N70:O70"/>
+    <mergeCell ref="N69:O69"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="F72:G72"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="F74:G74"/>
+    <mergeCell ref="H70:I70"/>
+    <mergeCell ref="H69:I69"/>
+    <mergeCell ref="H72:I72"/>
+    <mergeCell ref="H73:I73"/>
+    <mergeCell ref="H74:I74"/>
+    <mergeCell ref="J73:K73"/>
+    <mergeCell ref="J74:K74"/>
+    <mergeCell ref="L70:M70"/>
+    <mergeCell ref="L69:M69"/>
+    <mergeCell ref="L72:M72"/>
+    <mergeCell ref="L73:M73"/>
+    <mergeCell ref="L74:M74"/>
+    <mergeCell ref="N72:O72"/>
+    <mergeCell ref="N73:O73"/>
+    <mergeCell ref="N74:O74"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="A35:A38"/>
+    <mergeCell ref="A39:A42"/>
+    <mergeCell ref="A43:A46"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="J72:K72"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>